<commit_message>
updated freeman model training, plus minor changes
</commit_message>
<xml_diff>
--- a/datasets/cleaned/average_house_price.xlsx
+++ b/datasets/cleaned/average_house_price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aishachowdhury/Projects/aia-grad-hackathon/datasets/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F4916B-EDBB-474F-AE38-C75FC95741FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37AA9BB-F516-1043-A500-909BCA8A2D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{1B071781-4199-C044-8842-1EFFC136A2ED}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +159,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -182,11 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,9 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8495DD4A-2F1F-1E40-AEA2-5901725D64A4}">
   <dimension ref="A1:GO304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -534,55 +539,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:197" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="4">
         <v>2004</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="4">
         <v>2005</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="4">
         <v>2006</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="4">
         <v>2007</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="4">
         <v>2008</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="4">
         <v>2009</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="4">
         <v>2010</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="4">
         <v>2011</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="4">
         <v>2012</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="4">
         <v>2013</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="4">
         <v>2014</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="4">
         <v>2015</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="4">
         <v>2016</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="4">
         <v>2017</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="4">
         <v>2018</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="4">
         <v>2019</v>
       </c>
       <c r="R1" s="1"/>
@@ -768,53 +773,53 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>158176</v>
       </c>
-      <c r="C2" s="3">
-        <v>163360.91666666666</v>
-      </c>
-      <c r="D2" s="3">
-        <v>167853.25</v>
-      </c>
-      <c r="E2" s="3">
-        <v>184909.66666666666</v>
-      </c>
-      <c r="F2" s="3">
-        <v>187356.83333333334</v>
-      </c>
-      <c r="G2" s="3">
-        <v>156446.91666666666</v>
-      </c>
-      <c r="H2" s="3">
-        <v>166560.75</v>
-      </c>
-      <c r="I2" s="3">
-        <v>163465.08333333334</v>
-      </c>
-      <c r="J2" s="3">
-        <v>165863.91666666666</v>
-      </c>
-      <c r="K2" s="3">
-        <v>173733.66666666666</v>
-      </c>
-      <c r="L2" s="3">
-        <v>201172.25</v>
-      </c>
-      <c r="M2" s="3">
-        <v>233460.08333333334</v>
-      </c>
-      <c r="N2" s="3">
-        <v>273919.75</v>
-      </c>
-      <c r="O2" s="3">
-        <v>287734.83333333331</v>
-      </c>
-      <c r="P2" s="3">
-        <v>295196.66666666669</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>299294.16666666669</v>
+      <c r="C2" s="4">
+        <v>163361</v>
+      </c>
+      <c r="D2" s="4">
+        <v>167853</v>
+      </c>
+      <c r="E2" s="4">
+        <v>184910</v>
+      </c>
+      <c r="F2" s="4">
+        <v>187357</v>
+      </c>
+      <c r="G2" s="4">
+        <v>156447</v>
+      </c>
+      <c r="H2" s="4">
+        <v>166561</v>
+      </c>
+      <c r="I2" s="4">
+        <v>163465</v>
+      </c>
+      <c r="J2" s="4">
+        <v>165864</v>
+      </c>
+      <c r="K2" s="4">
+        <v>173734</v>
+      </c>
+      <c r="L2" s="4">
+        <v>201172</v>
+      </c>
+      <c r="M2" s="4">
+        <v>233460</v>
+      </c>
+      <c r="N2" s="4">
+        <v>273920</v>
+      </c>
+      <c r="O2" s="4">
+        <v>287735</v>
+      </c>
+      <c r="P2" s="4">
+        <v>295197</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>299294</v>
       </c>
       <c r="GO2" s="1"/>
     </row>
@@ -822,53 +827,53 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>271854.08333333331</v>
-      </c>
-      <c r="C3" s="3">
-        <v>279459.66666666669</v>
-      </c>
-      <c r="D3" s="3">
-        <v>291337.75</v>
-      </c>
-      <c r="E3" s="3">
-        <v>326915.41666666669</v>
-      </c>
-      <c r="F3" s="3">
-        <v>330023.33333333331</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="B3" s="4">
+        <v>271854</v>
+      </c>
+      <c r="C3" s="4">
+        <v>279460</v>
+      </c>
+      <c r="D3" s="4">
+        <v>291338</v>
+      </c>
+      <c r="E3" s="4">
+        <v>326915</v>
+      </c>
+      <c r="F3" s="4">
+        <v>330023</v>
+      </c>
+      <c r="G3" s="4">
         <v>299103</v>
       </c>
-      <c r="H3" s="3">
-        <v>333128.08333333331</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="H3" s="4">
+        <v>333128</v>
+      </c>
+      <c r="I3" s="4">
         <v>338978</v>
       </c>
-      <c r="J3" s="3">
-        <v>358627.41666666669</v>
-      </c>
-      <c r="K3" s="3">
-        <v>374770.58333333331</v>
-      </c>
-      <c r="L3" s="3">
-        <v>430363.33333333331</v>
-      </c>
-      <c r="M3" s="3">
-        <v>478688.08333333331</v>
-      </c>
-      <c r="N3" s="3">
-        <v>525939.5</v>
-      </c>
-      <c r="O3" s="3">
-        <v>538280.91666666663</v>
-      </c>
-      <c r="P3" s="3">
-        <v>533266.41666666663</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>519552.58333333331</v>
+      <c r="J3" s="4">
+        <v>358627</v>
+      </c>
+      <c r="K3" s="4">
+        <v>374771</v>
+      </c>
+      <c r="L3" s="4">
+        <v>430363</v>
+      </c>
+      <c r="M3" s="4">
+        <v>478688</v>
+      </c>
+      <c r="N3" s="4">
+        <v>525940</v>
+      </c>
+      <c r="O3" s="4">
+        <v>538281</v>
+      </c>
+      <c r="P3" s="4">
+        <v>533266</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>519553</v>
       </c>
       <c r="GO3" s="1"/>
     </row>
@@ -876,53 +881,53 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>179141.25</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="4">
+        <v>179141</v>
+      </c>
+      <c r="C4" s="4">
         <v>186512</v>
       </c>
-      <c r="D4" s="3">
-        <v>191831.25</v>
-      </c>
-      <c r="E4" s="3">
-        <v>208085.91666666666</v>
-      </c>
-      <c r="F4" s="3">
-        <v>210199.08333333334</v>
-      </c>
-      <c r="G4" s="3">
-        <v>189050.83333333334</v>
-      </c>
-      <c r="H4" s="3">
-        <v>200874.08333333334</v>
-      </c>
-      <c r="I4" s="3">
-        <v>200672.08333333334</v>
-      </c>
-      <c r="J4" s="3">
-        <v>202546.41666666666</v>
-      </c>
-      <c r="K4" s="3">
-        <v>213470.25</v>
-      </c>
-      <c r="L4" s="3">
-        <v>244459.58333333334</v>
-      </c>
-      <c r="M4" s="3">
-        <v>274209.25</v>
-      </c>
-      <c r="N4" s="3">
-        <v>321563.66666666669</v>
-      </c>
-      <c r="O4" s="3">
-        <v>335694.41666666669</v>
-      </c>
-      <c r="P4" s="3">
-        <v>342603.58333333331</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>337537.16666666669</v>
+      <c r="D4" s="4">
+        <v>191831</v>
+      </c>
+      <c r="E4" s="4">
+        <v>208086</v>
+      </c>
+      <c r="F4" s="4">
+        <v>210199</v>
+      </c>
+      <c r="G4" s="4">
+        <v>189051</v>
+      </c>
+      <c r="H4" s="4">
+        <v>200874</v>
+      </c>
+      <c r="I4" s="4">
+        <v>200672</v>
+      </c>
+      <c r="J4" s="4">
+        <v>202546</v>
+      </c>
+      <c r="K4" s="4">
+        <v>213470</v>
+      </c>
+      <c r="L4" s="4">
+        <v>244460</v>
+      </c>
+      <c r="M4" s="4">
+        <v>274209</v>
+      </c>
+      <c r="N4" s="4">
+        <v>321564</v>
+      </c>
+      <c r="O4" s="4">
+        <v>335694</v>
+      </c>
+      <c r="P4" s="4">
+        <v>342604</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>337537</v>
       </c>
       <c r="GO4" s="1"/>
     </row>
@@ -930,52 +935,52 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>236023.41666666666</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="4">
+        <v>236023</v>
+      </c>
+      <c r="C5" s="4">
         <v>241690</v>
       </c>
-      <c r="D5" s="3">
-        <v>253253.33333333334</v>
-      </c>
-      <c r="E5" s="3">
-        <v>286995.33333333331</v>
-      </c>
-      <c r="F5" s="3">
-        <v>292757.91666666669</v>
-      </c>
-      <c r="G5" s="3">
-        <v>264402.08333333331</v>
-      </c>
-      <c r="H5" s="3">
-        <v>289562.58333333331</v>
-      </c>
-      <c r="I5" s="3">
-        <v>298964.41666666669</v>
-      </c>
-      <c r="J5" s="3">
-        <v>314112.83333333331</v>
-      </c>
-      <c r="K5" s="3">
-        <v>339655.75</v>
-      </c>
-      <c r="L5" s="3">
-        <v>394687.41666666669</v>
-      </c>
-      <c r="M5" s="3">
-        <v>440951.75</v>
-      </c>
-      <c r="N5" s="3">
-        <v>489469.41666666669</v>
-      </c>
-      <c r="O5" s="3">
-        <v>487703.75</v>
-      </c>
-      <c r="P5" s="3">
-        <v>492845.33333333331</v>
-      </c>
-      <c r="Q5" s="3">
+      <c r="D5" s="4">
+        <v>253253</v>
+      </c>
+      <c r="E5" s="4">
+        <v>286995</v>
+      </c>
+      <c r="F5" s="4">
+        <v>292758</v>
+      </c>
+      <c r="G5" s="4">
+        <v>264402</v>
+      </c>
+      <c r="H5" s="4">
+        <v>289563</v>
+      </c>
+      <c r="I5" s="4">
+        <v>298964</v>
+      </c>
+      <c r="J5" s="4">
+        <v>314113</v>
+      </c>
+      <c r="K5" s="4">
+        <v>339656</v>
+      </c>
+      <c r="L5" s="4">
+        <v>394687</v>
+      </c>
+      <c r="M5" s="4">
+        <v>440952</v>
+      </c>
+      <c r="N5" s="4">
+        <v>489469</v>
+      </c>
+      <c r="O5" s="4">
+        <v>487704</v>
+      </c>
+      <c r="P5" s="4">
+        <v>492845</v>
+      </c>
+      <c r="Q5" s="4">
         <v>474172</v>
       </c>
       <c r="GO5" s="1"/>
@@ -984,53 +989,53 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>234462.66666666666</v>
-      </c>
-      <c r="C6" s="3">
-        <v>239786.25</v>
-      </c>
-      <c r="D6" s="3">
-        <v>249691.75</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6" s="4">
+        <v>234463</v>
+      </c>
+      <c r="C6" s="4">
+        <v>239786</v>
+      </c>
+      <c r="D6" s="4">
+        <v>249692</v>
+      </c>
+      <c r="E6" s="4">
         <v>277230</v>
       </c>
-      <c r="F6" s="3">
-        <v>277727.5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>249909.25</v>
-      </c>
-      <c r="H6" s="3">
-        <v>271049.08333333331</v>
-      </c>
-      <c r="I6" s="3">
-        <v>274874.5</v>
-      </c>
-      <c r="J6" s="3">
-        <v>282025.08333333331</v>
-      </c>
-      <c r="K6" s="3">
-        <v>296669.25</v>
-      </c>
-      <c r="L6" s="3">
-        <v>347857.33333333331</v>
-      </c>
-      <c r="M6" s="3">
-        <v>385681.5</v>
-      </c>
-      <c r="N6" s="3">
-        <v>428008.16666666669</v>
-      </c>
-      <c r="O6" s="3">
-        <v>441218.66666666669</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="F6" s="4">
+        <v>277728</v>
+      </c>
+      <c r="G6" s="4">
+        <v>249909</v>
+      </c>
+      <c r="H6" s="4">
+        <v>271049</v>
+      </c>
+      <c r="I6" s="4">
+        <v>274875</v>
+      </c>
+      <c r="J6" s="4">
+        <v>282025</v>
+      </c>
+      <c r="K6" s="4">
+        <v>296669</v>
+      </c>
+      <c r="L6" s="4">
+        <v>347857</v>
+      </c>
+      <c r="M6" s="4">
+        <v>385682</v>
+      </c>
+      <c r="N6" s="4">
+        <v>428008</v>
+      </c>
+      <c r="O6" s="4">
+        <v>441219</v>
+      </c>
+      <c r="P6" s="4">
         <v>443410</v>
       </c>
-      <c r="Q6" s="3">
-        <v>437700.33333333331</v>
+      <c r="Q6" s="4">
+        <v>437700</v>
       </c>
       <c r="GO6" s="1"/>
     </row>
@@ -1038,53 +1043,53 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>351847.75</v>
-      </c>
-      <c r="C7" s="3">
-        <v>368345.08333333331</v>
-      </c>
-      <c r="D7" s="3">
-        <v>394819.5</v>
-      </c>
-      <c r="E7" s="3">
-        <v>466485.58333333331</v>
-      </c>
-      <c r="F7" s="3">
-        <v>501223.33333333331</v>
-      </c>
-      <c r="G7" s="3">
-        <v>454627.91666666669</v>
-      </c>
-      <c r="H7" s="3">
-        <v>513221.08333333331</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="B7" s="4">
+        <v>351848</v>
+      </c>
+      <c r="C7" s="4">
+        <v>368345</v>
+      </c>
+      <c r="D7" s="4">
+        <v>394820</v>
+      </c>
+      <c r="E7" s="4">
+        <v>466486</v>
+      </c>
+      <c r="F7" s="4">
+        <v>501223</v>
+      </c>
+      <c r="G7" s="4">
+        <v>454628</v>
+      </c>
+      <c r="H7" s="4">
+        <v>513221</v>
+      </c>
+      <c r="I7" s="4">
         <v>554393</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="4">
         <v>586166</v>
       </c>
-      <c r="K7" s="3">
-        <v>667447.58333333337</v>
-      </c>
-      <c r="L7" s="3">
-        <v>756486.33333333337</v>
-      </c>
-      <c r="M7" s="3">
-        <v>787440.91666666663</v>
-      </c>
-      <c r="N7" s="3">
+      <c r="K7" s="4">
+        <v>667448</v>
+      </c>
+      <c r="L7" s="4">
+        <v>756486</v>
+      </c>
+      <c r="M7" s="4">
+        <v>787441</v>
+      </c>
+      <c r="N7" s="4">
         <v>807119</v>
       </c>
-      <c r="O7" s="3">
-        <v>839347.5</v>
-      </c>
-      <c r="P7" s="3">
-        <v>842410.5</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>838532.91666666663</v>
+      <c r="O7" s="4">
+        <v>839348</v>
+      </c>
+      <c r="P7" s="4">
+        <v>842411</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>838533</v>
       </c>
       <c r="GO7" s="1"/>
     </row>
@@ -1092,53 +1097,53 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>301032.83333333331</v>
-      </c>
-      <c r="C8" s="3">
-        <v>311783.66666666669</v>
-      </c>
-      <c r="D8" s="3">
-        <v>338518.58333333331</v>
-      </c>
-      <c r="E8" s="3">
-        <v>433838.41666666669</v>
-      </c>
-      <c r="F8" s="3">
-        <v>427296.83333333331</v>
-      </c>
-      <c r="G8" s="3">
-        <v>383417.83333333331</v>
-      </c>
-      <c r="H8" s="3">
-        <v>453662.83333333331</v>
-      </c>
-      <c r="I8" s="3">
-        <v>463930.83333333331</v>
-      </c>
-      <c r="J8" s="3">
-        <v>525327.5</v>
-      </c>
-      <c r="K8" s="3">
-        <v>570008.66666666663</v>
-      </c>
-      <c r="L8" s="3">
-        <v>709385.41666666663</v>
-      </c>
-      <c r="M8" s="3">
-        <v>760253.16666666663</v>
-      </c>
-      <c r="N8" s="3">
-        <v>818315.5</v>
-      </c>
-      <c r="O8" s="3">
-        <v>849790.16666666663</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="B8" s="4">
+        <v>301033</v>
+      </c>
+      <c r="C8" s="4">
+        <v>311784</v>
+      </c>
+      <c r="D8" s="4">
+        <v>338519</v>
+      </c>
+      <c r="E8" s="4">
+        <v>433838</v>
+      </c>
+      <c r="F8" s="4">
+        <v>427297</v>
+      </c>
+      <c r="G8" s="4">
+        <v>383418</v>
+      </c>
+      <c r="H8" s="4">
+        <v>453663</v>
+      </c>
+      <c r="I8" s="4">
+        <v>463931</v>
+      </c>
+      <c r="J8" s="4">
+        <v>525328</v>
+      </c>
+      <c r="K8" s="4">
+        <v>570009</v>
+      </c>
+      <c r="L8" s="4">
+        <v>709385</v>
+      </c>
+      <c r="M8" s="4">
+        <v>760253</v>
+      </c>
+      <c r="N8" s="4">
+        <v>818316</v>
+      </c>
+      <c r="O8" s="4">
+        <v>849790</v>
+      </c>
+      <c r="P8" s="4">
         <v>784809</v>
       </c>
-      <c r="Q8" s="3">
-        <v>786983.08333333337</v>
+      <c r="Q8" s="4">
+        <v>786983</v>
       </c>
       <c r="GO8" s="1"/>
     </row>
@@ -1146,53 +1151,53 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>198588.66666666666</v>
-      </c>
-      <c r="C9" s="3">
-        <v>204407.33333333334</v>
-      </c>
-      <c r="D9" s="3">
-        <v>212111.25</v>
-      </c>
-      <c r="E9" s="3">
-        <v>233665.75</v>
-      </c>
-      <c r="F9" s="3">
-        <v>235998.5</v>
-      </c>
-      <c r="G9" s="3">
-        <v>203706.41666666666</v>
-      </c>
-      <c r="H9" s="3">
-        <v>218639.83333333334</v>
-      </c>
-      <c r="I9" s="3">
-        <v>215427.58333333334</v>
-      </c>
-      <c r="J9" s="3">
-        <v>221817.08333333334</v>
-      </c>
-      <c r="K9" s="3">
-        <v>234439.83333333334</v>
-      </c>
-      <c r="L9" s="3">
-        <v>274827.41666666669</v>
-      </c>
-      <c r="M9" s="3">
-        <v>307064.16666666669</v>
-      </c>
-      <c r="N9" s="3">
-        <v>355846.66666666669</v>
-      </c>
-      <c r="O9" s="3">
-        <v>372554.41666666669</v>
-      </c>
-      <c r="P9" s="3">
-        <v>370298.41666666669</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>365350.83333333331</v>
+      <c r="B9" s="4">
+        <v>198589</v>
+      </c>
+      <c r="C9" s="4">
+        <v>204407</v>
+      </c>
+      <c r="D9" s="4">
+        <v>212111</v>
+      </c>
+      <c r="E9" s="4">
+        <v>233666</v>
+      </c>
+      <c r="F9" s="4">
+        <v>235999</v>
+      </c>
+      <c r="G9" s="4">
+        <v>203706</v>
+      </c>
+      <c r="H9" s="4">
+        <v>218640</v>
+      </c>
+      <c r="I9" s="4">
+        <v>215428</v>
+      </c>
+      <c r="J9" s="4">
+        <v>221817</v>
+      </c>
+      <c r="K9" s="4">
+        <v>234440</v>
+      </c>
+      <c r="L9" s="4">
+        <v>274827</v>
+      </c>
+      <c r="M9" s="4">
+        <v>307064</v>
+      </c>
+      <c r="N9" s="4">
+        <v>355847</v>
+      </c>
+      <c r="O9" s="4">
+        <v>372554</v>
+      </c>
+      <c r="P9" s="4">
+        <v>370298</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>365351</v>
       </c>
       <c r="GO9" s="1"/>
     </row>
@@ -1200,53 +1205,53 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>241038.58333333334</v>
-      </c>
-      <c r="C10" s="3">
-        <v>244871.91666666666</v>
-      </c>
-      <c r="D10" s="3">
-        <v>260206.25</v>
-      </c>
-      <c r="E10" s="3">
-        <v>293783.83333333331</v>
-      </c>
-      <c r="F10" s="3">
-        <v>295324.5</v>
-      </c>
-      <c r="G10" s="3">
-        <v>264041.91666666669</v>
-      </c>
-      <c r="H10" s="3">
-        <v>292825.75</v>
-      </c>
-      <c r="I10" s="3">
-        <v>302306.91666666669</v>
-      </c>
-      <c r="J10" s="3">
-        <v>318697.75</v>
-      </c>
-      <c r="K10" s="3">
-        <v>338088.83333333331</v>
-      </c>
-      <c r="L10" s="3">
-        <v>400039.16666666669</v>
-      </c>
-      <c r="M10" s="3">
-        <v>438310.58333333331</v>
-      </c>
-      <c r="N10" s="3">
-        <v>476440.66666666669</v>
-      </c>
-      <c r="O10" s="3">
-        <v>484592.08333333331</v>
-      </c>
-      <c r="P10" s="3">
-        <v>480050.58333333331</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>472601.41666666669</v>
+      <c r="B10" s="4">
+        <v>241039</v>
+      </c>
+      <c r="C10" s="4">
+        <v>244872</v>
+      </c>
+      <c r="D10" s="4">
+        <v>260206</v>
+      </c>
+      <c r="E10" s="4">
+        <v>293784</v>
+      </c>
+      <c r="F10" s="4">
+        <v>295325</v>
+      </c>
+      <c r="G10" s="4">
+        <v>264042</v>
+      </c>
+      <c r="H10" s="4">
+        <v>292826</v>
+      </c>
+      <c r="I10" s="4">
+        <v>302307</v>
+      </c>
+      <c r="J10" s="4">
+        <v>318698</v>
+      </c>
+      <c r="K10" s="4">
+        <v>338089</v>
+      </c>
+      <c r="L10" s="4">
+        <v>400039</v>
+      </c>
+      <c r="M10" s="4">
+        <v>438311</v>
+      </c>
+      <c r="N10" s="4">
+        <v>476441</v>
+      </c>
+      <c r="O10" s="4">
+        <v>484592</v>
+      </c>
+      <c r="P10" s="4">
+        <v>480051</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>472601</v>
       </c>
       <c r="GO10" s="1"/>
     </row>
@@ -1254,53 +1259,53 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>205848.16666666666</v>
-      </c>
-      <c r="C11" s="3">
-        <v>212548.66666666666</v>
-      </c>
-      <c r="D11" s="3">
-        <v>219541.66666666666</v>
-      </c>
-      <c r="E11" s="3">
-        <v>243911.66666666666</v>
-      </c>
-      <c r="F11" s="3">
-        <v>245839.33333333334</v>
-      </c>
-      <c r="G11" s="3">
-        <v>221993.25</v>
-      </c>
-      <c r="H11" s="3">
-        <v>242127.41666666666</v>
-      </c>
-      <c r="I11" s="3">
-        <v>241991.25</v>
-      </c>
-      <c r="J11" s="3">
-        <v>247667.25</v>
-      </c>
-      <c r="K11" s="3">
-        <v>261604.41666666666</v>
-      </c>
-      <c r="L11" s="3">
-        <v>294515.66666666669</v>
-      </c>
-      <c r="M11" s="3">
-        <v>335503.66666666669</v>
-      </c>
-      <c r="N11" s="3">
-        <v>385489.75</v>
-      </c>
-      <c r="O11" s="3">
-        <v>395929.16666666669</v>
-      </c>
-      <c r="P11" s="3">
-        <v>396631.66666666669</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>393185.91666666669</v>
+      <c r="B11" s="4">
+        <v>205848</v>
+      </c>
+      <c r="C11" s="4">
+        <v>212549</v>
+      </c>
+      <c r="D11" s="4">
+        <v>219542</v>
+      </c>
+      <c r="E11" s="4">
+        <v>243912</v>
+      </c>
+      <c r="F11" s="4">
+        <v>245839</v>
+      </c>
+      <c r="G11" s="4">
+        <v>221993</v>
+      </c>
+      <c r="H11" s="4">
+        <v>242127</v>
+      </c>
+      <c r="I11" s="4">
+        <v>241991</v>
+      </c>
+      <c r="J11" s="4">
+        <v>247667</v>
+      </c>
+      <c r="K11" s="4">
+        <v>261604</v>
+      </c>
+      <c r="L11" s="4">
+        <v>294516</v>
+      </c>
+      <c r="M11" s="4">
+        <v>335504</v>
+      </c>
+      <c r="N11" s="4">
+        <v>385490</v>
+      </c>
+      <c r="O11" s="4">
+        <v>395929</v>
+      </c>
+      <c r="P11" s="4">
+        <v>396632</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>393186</v>
       </c>
       <c r="GO11" s="1"/>
     </row>
@@ -1308,53 +1313,53 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>186893.66666666666</v>
-      </c>
-      <c r="C12" s="3">
-        <v>196343.91666666666</v>
-      </c>
-      <c r="D12" s="3">
-        <v>207167.33333333334</v>
-      </c>
-      <c r="E12" s="3">
-        <v>228861.91666666666</v>
-      </c>
-      <c r="F12" s="3">
-        <v>231136.08333333334</v>
-      </c>
-      <c r="G12" s="3">
-        <v>210322.58333333334</v>
-      </c>
-      <c r="H12" s="3">
-        <v>229069.5</v>
-      </c>
-      <c r="I12" s="3">
-        <v>229295.41666666666</v>
-      </c>
-      <c r="J12" s="3">
-        <v>236980.83333333334</v>
-      </c>
-      <c r="K12" s="3">
-        <v>253399.25</v>
-      </c>
-      <c r="L12" s="3">
-        <v>298351.58333333331</v>
-      </c>
-      <c r="M12" s="3">
-        <v>331848.91666666669</v>
-      </c>
-      <c r="N12" s="3">
-        <v>372737.75</v>
-      </c>
-      <c r="O12" s="3">
-        <v>391749.83333333331</v>
-      </c>
-      <c r="P12" s="3">
-        <v>388344.41666666669</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>391435.16666666669</v>
+      <c r="B12" s="4">
+        <v>186894</v>
+      </c>
+      <c r="C12" s="4">
+        <v>196344</v>
+      </c>
+      <c r="D12" s="4">
+        <v>207167</v>
+      </c>
+      <c r="E12" s="4">
+        <v>228862</v>
+      </c>
+      <c r="F12" s="4">
+        <v>231136</v>
+      </c>
+      <c r="G12" s="4">
+        <v>210323</v>
+      </c>
+      <c r="H12" s="4">
+        <v>229070</v>
+      </c>
+      <c r="I12" s="4">
+        <v>229295</v>
+      </c>
+      <c r="J12" s="4">
+        <v>236981</v>
+      </c>
+      <c r="K12" s="4">
+        <v>253399</v>
+      </c>
+      <c r="L12" s="4">
+        <v>298352</v>
+      </c>
+      <c r="M12" s="4">
+        <v>331849</v>
+      </c>
+      <c r="N12" s="4">
+        <v>372738</v>
+      </c>
+      <c r="O12" s="4">
+        <v>391750</v>
+      </c>
+      <c r="P12" s="4">
+        <v>388344</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>391435</v>
       </c>
       <c r="GO12" s="1"/>
     </row>
@@ -1362,53 +1367,53 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>217677.25</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="4">
+        <v>217677</v>
+      </c>
+      <c r="C13" s="4">
         <v>227937</v>
       </c>
-      <c r="D13" s="3">
-        <v>253254.5</v>
-      </c>
-      <c r="E13" s="3">
-        <v>290396.83333333331</v>
-      </c>
-      <c r="F13" s="3">
-        <v>311770.5</v>
-      </c>
-      <c r="G13" s="3">
-        <v>282240.75</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="D13" s="4">
+        <v>253255</v>
+      </c>
+      <c r="E13" s="4">
+        <v>290397</v>
+      </c>
+      <c r="F13" s="4">
+        <v>311771</v>
+      </c>
+      <c r="G13" s="4">
+        <v>282241</v>
+      </c>
+      <c r="H13" s="4">
         <v>300491</v>
       </c>
-      <c r="I13" s="3">
-        <v>308698.33333333331</v>
-      </c>
-      <c r="J13" s="3">
-        <v>325492.66666666669</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="I13" s="4">
+        <v>308698</v>
+      </c>
+      <c r="J13" s="4">
+        <v>325493</v>
+      </c>
+      <c r="K13" s="4">
         <v>372669</v>
       </c>
-      <c r="L13" s="3">
-        <v>456388.5</v>
-      </c>
-      <c r="M13" s="3">
-        <v>506799.08333333331</v>
-      </c>
-      <c r="N13" s="3">
-        <v>537746.33333333337</v>
-      </c>
-      <c r="O13" s="3">
-        <v>549005.5</v>
-      </c>
-      <c r="P13" s="3">
-        <v>544640.41666666663</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>558008.83333333337</v>
+      <c r="L13" s="4">
+        <v>456389</v>
+      </c>
+      <c r="M13" s="4">
+        <v>506799</v>
+      </c>
+      <c r="N13" s="4">
+        <v>537746</v>
+      </c>
+      <c r="O13" s="4">
+        <v>549006</v>
+      </c>
+      <c r="P13" s="4">
+        <v>544640</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>558009</v>
       </c>
       <c r="GO13" s="1"/>
     </row>
@@ -1416,53 +1421,53 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>343381</v>
       </c>
-      <c r="C14" s="3">
-        <v>362575.58333333331</v>
-      </c>
-      <c r="D14" s="3">
-        <v>397586.41666666669</v>
-      </c>
-      <c r="E14" s="3">
-        <v>474140.75</v>
-      </c>
-      <c r="F14" s="3">
-        <v>474947.83333333331</v>
-      </c>
-      <c r="G14" s="3">
-        <v>435456.58333333331</v>
-      </c>
-      <c r="H14" s="3">
-        <v>502256.83333333331</v>
-      </c>
-      <c r="I14" s="3">
-        <v>518573.75</v>
-      </c>
-      <c r="J14" s="3">
+      <c r="C14" s="4">
+        <v>362576</v>
+      </c>
+      <c r="D14" s="4">
+        <v>397586</v>
+      </c>
+      <c r="E14" s="4">
+        <v>474141</v>
+      </c>
+      <c r="F14" s="4">
+        <v>474948</v>
+      </c>
+      <c r="G14" s="4">
+        <v>435457</v>
+      </c>
+      <c r="H14" s="4">
+        <v>502257</v>
+      </c>
+      <c r="I14" s="4">
+        <v>518574</v>
+      </c>
+      <c r="J14" s="4">
         <v>567082</v>
       </c>
-      <c r="K14" s="3">
-        <v>631529.08333333337</v>
-      </c>
-      <c r="L14" s="3">
-        <v>721099.75</v>
-      </c>
-      <c r="M14" s="3">
-        <v>760833.75</v>
-      </c>
-      <c r="N14" s="3">
-        <v>755097.5</v>
-      </c>
-      <c r="O14" s="3">
-        <v>756900.41666666663</v>
-      </c>
-      <c r="P14" s="3">
-        <v>725525.33333333337</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>720648.66666666663</v>
+      <c r="K14" s="4">
+        <v>631529</v>
+      </c>
+      <c r="L14" s="4">
+        <v>721100</v>
+      </c>
+      <c r="M14" s="4">
+        <v>760834</v>
+      </c>
+      <c r="N14" s="4">
+        <v>755098</v>
+      </c>
+      <c r="O14" s="4">
+        <v>756900</v>
+      </c>
+      <c r="P14" s="4">
+        <v>725525</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>720649</v>
       </c>
       <c r="GO14" s="1"/>
     </row>
@@ -1470,53 +1475,53 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>236265.16666666666</v>
-      </c>
-      <c r="C15" s="3">
-        <v>245820.66666666666</v>
-      </c>
-      <c r="D15" s="3">
-        <v>263920.83333333331</v>
-      </c>
-      <c r="E15" s="3">
-        <v>305509.41666666669</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="B15" s="4">
+        <v>236265</v>
+      </c>
+      <c r="C15" s="4">
+        <v>245821</v>
+      </c>
+      <c r="D15" s="4">
+        <v>263921</v>
+      </c>
+      <c r="E15" s="4">
+        <v>305509</v>
+      </c>
+      <c r="F15" s="4">
         <v>303396</v>
       </c>
-      <c r="G15" s="3">
-        <v>276214.08333333331</v>
-      </c>
-      <c r="H15" s="3">
-        <v>314479.83333333331</v>
-      </c>
-      <c r="I15" s="3">
-        <v>326468.25</v>
-      </c>
-      <c r="J15" s="3">
-        <v>339685.91666666669</v>
-      </c>
-      <c r="K15" s="3">
-        <v>372233.66666666669</v>
-      </c>
-      <c r="L15" s="3">
-        <v>435807.83333333331</v>
-      </c>
-      <c r="M15" s="3">
-        <v>480636.08333333331</v>
-      </c>
-      <c r="N15" s="3">
-        <v>527676.66666666663</v>
-      </c>
-      <c r="O15" s="3">
-        <v>557307.08333333337</v>
-      </c>
-      <c r="P15" s="3">
-        <v>551560.66666666663</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>548686.91666666663</v>
+      <c r="G15" s="4">
+        <v>276214</v>
+      </c>
+      <c r="H15" s="4">
+        <v>314480</v>
+      </c>
+      <c r="I15" s="4">
+        <v>326468</v>
+      </c>
+      <c r="J15" s="4">
+        <v>339686</v>
+      </c>
+      <c r="K15" s="4">
+        <v>372234</v>
+      </c>
+      <c r="L15" s="4">
+        <v>435808</v>
+      </c>
+      <c r="M15" s="4">
+        <v>480636</v>
+      </c>
+      <c r="N15" s="4">
+        <v>527677</v>
+      </c>
+      <c r="O15" s="4">
+        <v>557307</v>
+      </c>
+      <c r="P15" s="4">
+        <v>551561</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>548687</v>
       </c>
       <c r="GO15" s="1"/>
     </row>
@@ -1524,53 +1529,53 @@
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>252291.83333333334</v>
-      </c>
-      <c r="C16" s="3">
-        <v>255332.66666666666</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="B16" s="4">
+        <v>252292</v>
+      </c>
+      <c r="C16" s="4">
+        <v>255333</v>
+      </c>
+      <c r="D16" s="4">
         <v>265448</v>
       </c>
-      <c r="E16" s="3">
-        <v>293492.16666666669</v>
-      </c>
-      <c r="F16" s="3">
-        <v>294650.16666666669</v>
-      </c>
-      <c r="G16" s="3">
-        <v>263036.16666666669</v>
-      </c>
-      <c r="H16" s="3">
-        <v>292166.08333333331</v>
-      </c>
-      <c r="I16" s="3">
-        <v>296477.83333333331</v>
-      </c>
-      <c r="J16" s="3">
-        <v>304904.5</v>
-      </c>
-      <c r="K16" s="3">
-        <v>319397.66666666669</v>
-      </c>
-      <c r="L16" s="3">
-        <v>360795.83333333331</v>
-      </c>
-      <c r="M16" s="3">
-        <v>408604.58333333331</v>
-      </c>
-      <c r="N16" s="3">
-        <v>453862.33333333331</v>
-      </c>
-      <c r="O16" s="3">
-        <v>470763.41666666669</v>
-      </c>
-      <c r="P16" s="3">
-        <v>465907.5</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>449370.66666666669</v>
+      <c r="E16" s="4">
+        <v>293492</v>
+      </c>
+      <c r="F16" s="4">
+        <v>294650</v>
+      </c>
+      <c r="G16" s="4">
+        <v>263036</v>
+      </c>
+      <c r="H16" s="4">
+        <v>292166</v>
+      </c>
+      <c r="I16" s="4">
+        <v>296478</v>
+      </c>
+      <c r="J16" s="4">
+        <v>304905</v>
+      </c>
+      <c r="K16" s="4">
+        <v>319398</v>
+      </c>
+      <c r="L16" s="4">
+        <v>360796</v>
+      </c>
+      <c r="M16" s="4">
+        <v>408605</v>
+      </c>
+      <c r="N16" s="4">
+        <v>453862</v>
+      </c>
+      <c r="O16" s="4">
+        <v>470763</v>
+      </c>
+      <c r="P16" s="4">
+        <v>465908</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>449371</v>
       </c>
       <c r="GO16" s="1"/>
     </row>
@@ -1578,53 +1583,53 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>195992.41666666666</v>
-      </c>
-      <c r="C17" s="3">
-        <v>204047.33333333334</v>
-      </c>
-      <c r="D17" s="3">
-        <v>211316.5</v>
-      </c>
-      <c r="E17" s="3">
-        <v>233534.83333333334</v>
-      </c>
-      <c r="F17" s="3">
-        <v>231473.75</v>
-      </c>
-      <c r="G17" s="3">
-        <v>205962.08333333334</v>
-      </c>
-      <c r="H17" s="3">
-        <v>220413.25</v>
-      </c>
-      <c r="I17" s="3">
-        <v>219558.83333333334</v>
-      </c>
-      <c r="J17" s="3">
-        <v>221601.91666666666</v>
-      </c>
-      <c r="K17" s="3">
-        <v>226428.83333333334</v>
-      </c>
-      <c r="L17" s="3">
-        <v>259267.25</v>
-      </c>
-      <c r="M17" s="3">
-        <v>291844.83333333331</v>
-      </c>
-      <c r="N17" s="3">
-        <v>341803.91666666669</v>
-      </c>
-      <c r="O17" s="3">
-        <v>360479.33333333331</v>
-      </c>
-      <c r="P17" s="3">
-        <v>370248.91666666669</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>364822.16666666669</v>
+      <c r="B17" s="4">
+        <v>195992</v>
+      </c>
+      <c r="C17" s="4">
+        <v>204047</v>
+      </c>
+      <c r="D17" s="4">
+        <v>211317</v>
+      </c>
+      <c r="E17" s="4">
+        <v>233535</v>
+      </c>
+      <c r="F17" s="4">
+        <v>231474</v>
+      </c>
+      <c r="G17" s="4">
+        <v>205962</v>
+      </c>
+      <c r="H17" s="4">
+        <v>220413</v>
+      </c>
+      <c r="I17" s="4">
+        <v>219559</v>
+      </c>
+      <c r="J17" s="4">
+        <v>221602</v>
+      </c>
+      <c r="K17" s="4">
+        <v>226429</v>
+      </c>
+      <c r="L17" s="4">
+        <v>259267</v>
+      </c>
+      <c r="M17" s="4">
+        <v>291845</v>
+      </c>
+      <c r="N17" s="4">
+        <v>341804</v>
+      </c>
+      <c r="O17" s="4">
+        <v>360479</v>
+      </c>
+      <c r="P17" s="4">
+        <v>370249</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>364822</v>
       </c>
       <c r="GO17" s="1"/>
     </row>
@@ -1632,53 +1637,53 @@
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
-        <v>215696.08333333334</v>
-      </c>
-      <c r="C18" s="3">
-        <v>222899.83333333334</v>
-      </c>
-      <c r="D18" s="3">
-        <v>231405.16666666666</v>
-      </c>
-      <c r="E18" s="3">
-        <v>253838.58333333334</v>
-      </c>
-      <c r="F18" s="3">
-        <v>255580.25</v>
-      </c>
-      <c r="G18" s="3">
-        <v>228275.83333333334</v>
-      </c>
-      <c r="H18" s="3">
-        <v>247991.58333333334</v>
-      </c>
-      <c r="I18" s="3">
-        <v>251781.66666666666</v>
-      </c>
-      <c r="J18" s="3">
-        <v>260476.5</v>
-      </c>
-      <c r="K18" s="3">
-        <v>270594.75</v>
-      </c>
-      <c r="L18" s="3">
-        <v>305781.91666666669</v>
-      </c>
-      <c r="M18" s="3">
-        <v>352748.41666666669</v>
-      </c>
-      <c r="N18" s="3">
-        <v>400791.41666666669</v>
-      </c>
-      <c r="O18" s="3">
-        <v>413586.66666666669</v>
-      </c>
-      <c r="P18" s="3">
+      <c r="B18" s="4">
+        <v>215696</v>
+      </c>
+      <c r="C18" s="4">
+        <v>222900</v>
+      </c>
+      <c r="D18" s="4">
+        <v>231405</v>
+      </c>
+      <c r="E18" s="4">
+        <v>253839</v>
+      </c>
+      <c r="F18" s="4">
+        <v>255580</v>
+      </c>
+      <c r="G18" s="4">
+        <v>228276</v>
+      </c>
+      <c r="H18" s="4">
+        <v>247992</v>
+      </c>
+      <c r="I18" s="4">
+        <v>251782</v>
+      </c>
+      <c r="J18" s="4">
+        <v>260477</v>
+      </c>
+      <c r="K18" s="4">
+        <v>270595</v>
+      </c>
+      <c r="L18" s="4">
+        <v>305782</v>
+      </c>
+      <c r="M18" s="4">
+        <v>352748</v>
+      </c>
+      <c r="N18" s="4">
+        <v>400791</v>
+      </c>
+      <c r="O18" s="4">
+        <v>413587</v>
+      </c>
+      <c r="P18" s="4">
         <v>410266</v>
       </c>
-      <c r="Q18" s="3">
-        <v>404784.66666666669</v>
+      <c r="Q18" s="4">
+        <v>404785</v>
       </c>
       <c r="GO18" s="1"/>
     </row>
@@ -1686,53 +1691,53 @@
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>215827.08333333334</v>
-      </c>
-      <c r="C19" s="3">
-        <v>222920.91666666666</v>
-      </c>
-      <c r="D19" s="3">
-        <v>237044.58333333334</v>
-      </c>
-      <c r="E19" s="3">
-        <v>260228.16666666666</v>
-      </c>
-      <c r="F19" s="3">
-        <v>262945.58333333331</v>
-      </c>
-      <c r="G19" s="3">
-        <v>236242.66666666666</v>
-      </c>
-      <c r="H19" s="3">
-        <v>257449.58333333334</v>
-      </c>
-      <c r="I19" s="3">
-        <v>264605.33333333331</v>
-      </c>
-      <c r="J19" s="3">
-        <v>267958.16666666669</v>
-      </c>
-      <c r="K19" s="3">
-        <v>290577.33333333331</v>
-      </c>
-      <c r="L19" s="3">
-        <v>324525.83333333331</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="B19" s="4">
+        <v>215827</v>
+      </c>
+      <c r="C19" s="4">
+        <v>222921</v>
+      </c>
+      <c r="D19" s="4">
+        <v>237045</v>
+      </c>
+      <c r="E19" s="4">
+        <v>260228</v>
+      </c>
+      <c r="F19" s="4">
+        <v>262946</v>
+      </c>
+      <c r="G19" s="4">
+        <v>236243</v>
+      </c>
+      <c r="H19" s="4">
+        <v>257450</v>
+      </c>
+      <c r="I19" s="4">
+        <v>264605</v>
+      </c>
+      <c r="J19" s="4">
+        <v>267958</v>
+      </c>
+      <c r="K19" s="4">
+        <v>290577</v>
+      </c>
+      <c r="L19" s="4">
+        <v>324526</v>
+      </c>
+      <c r="M19" s="4">
         <v>351438</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="4">
         <v>386462</v>
       </c>
-      <c r="O19" s="3">
-        <v>400904.5</v>
-      </c>
-      <c r="P19" s="3">
-        <v>396631.08333333331</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>401851.33333333331</v>
+      <c r="O19" s="4">
+        <v>400905</v>
+      </c>
+      <c r="P19" s="4">
+        <v>396631</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>401851</v>
       </c>
       <c r="GO19" s="1"/>
     </row>
@@ -1740,53 +1745,53 @@
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>285947.08333333331</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="4">
+        <v>285947</v>
+      </c>
+      <c r="C20" s="4">
         <v>295082</v>
       </c>
-      <c r="D20" s="3">
-        <v>319644.83333333331</v>
-      </c>
-      <c r="E20" s="3">
-        <v>385665.5</v>
-      </c>
-      <c r="F20" s="3">
-        <v>386792.41666666669</v>
-      </c>
-      <c r="G20" s="3">
-        <v>345284.33333333331</v>
-      </c>
-      <c r="H20" s="3">
-        <v>398055.08333333331</v>
-      </c>
-      <c r="I20" s="3">
-        <v>424103.75</v>
-      </c>
-      <c r="J20" s="3">
-        <v>442090.25</v>
-      </c>
-      <c r="K20" s="3">
-        <v>495766.25</v>
-      </c>
-      <c r="L20" s="3">
-        <v>585171.33333333337</v>
-      </c>
-      <c r="M20" s="3">
-        <v>643147.83333333337</v>
-      </c>
-      <c r="N20" s="3">
+      <c r="D20" s="4">
+        <v>319645</v>
+      </c>
+      <c r="E20" s="4">
+        <v>385666</v>
+      </c>
+      <c r="F20" s="4">
+        <v>386792</v>
+      </c>
+      <c r="G20" s="4">
+        <v>345284</v>
+      </c>
+      <c r="H20" s="4">
+        <v>398055</v>
+      </c>
+      <c r="I20" s="4">
+        <v>424104</v>
+      </c>
+      <c r="J20" s="4">
+        <v>442090</v>
+      </c>
+      <c r="K20" s="4">
+        <v>495766</v>
+      </c>
+      <c r="L20" s="4">
+        <v>585171</v>
+      </c>
+      <c r="M20" s="4">
+        <v>643148</v>
+      </c>
+      <c r="N20" s="4">
         <v>642137</v>
       </c>
-      <c r="O20" s="3">
-        <v>650114.66666666663</v>
-      </c>
-      <c r="P20" s="3">
-        <v>649824.08333333337</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>634966.83333333337</v>
+      <c r="O20" s="4">
+        <v>650115</v>
+      </c>
+      <c r="P20" s="4">
+        <v>649824</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>634967</v>
       </c>
       <c r="GO20" s="1"/>
     </row>
@@ -1794,53 +1799,53 @@
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>512186.66666666669</v>
-      </c>
-      <c r="C21" s="3">
-        <v>520206.25</v>
-      </c>
-      <c r="D21" s="3">
-        <v>598007.5</v>
-      </c>
-      <c r="E21" s="3">
-        <v>746679.25</v>
-      </c>
-      <c r="F21" s="3">
-        <v>784834.58333333337</v>
-      </c>
-      <c r="G21" s="3">
-        <v>705187.5</v>
-      </c>
-      <c r="H21" s="3">
-        <v>837314.91666666663</v>
-      </c>
-      <c r="I21" s="3">
-        <v>908565.08333333337</v>
-      </c>
-      <c r="J21" s="3">
-        <v>1009044.8333333334</v>
-      </c>
-      <c r="K21" s="3">
-        <v>1126572.8333333333</v>
-      </c>
-      <c r="L21" s="3">
-        <v>1288405.6666666667</v>
-      </c>
-      <c r="M21" s="3">
-        <v>1302102.75</v>
-      </c>
-      <c r="N21" s="3">
-        <v>1276235.1666666667</v>
-      </c>
-      <c r="O21" s="3">
-        <v>1344539.75</v>
-      </c>
-      <c r="P21" s="3">
-        <v>1363880.0833333333</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>1247124.5833333333</v>
+      <c r="B21" s="4">
+        <v>512187</v>
+      </c>
+      <c r="C21" s="4">
+        <v>520206</v>
+      </c>
+      <c r="D21" s="4">
+        <v>598008</v>
+      </c>
+      <c r="E21" s="4">
+        <v>746679</v>
+      </c>
+      <c r="F21" s="4">
+        <v>784835</v>
+      </c>
+      <c r="G21" s="4">
+        <v>705188</v>
+      </c>
+      <c r="H21" s="4">
+        <v>837315</v>
+      </c>
+      <c r="I21" s="4">
+        <v>908565</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1009045</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1126573</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1288406</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1302103</v>
+      </c>
+      <c r="N21" s="4">
+        <v>1276235</v>
+      </c>
+      <c r="O21" s="4">
+        <v>1344540</v>
+      </c>
+      <c r="P21" s="4">
+        <v>1363880</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>1247125</v>
       </c>
       <c r="GO21" s="1"/>
     </row>
@@ -1848,53 +1853,53 @@
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>246424.08333333334</v>
-      </c>
-      <c r="C22" s="3">
-        <v>251156.33333333334</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="B22" s="4">
+        <v>246424</v>
+      </c>
+      <c r="C22" s="4">
+        <v>251156</v>
+      </c>
+      <c r="D22" s="4">
         <v>264667</v>
       </c>
-      <c r="E22" s="3">
-        <v>306229.33333333331</v>
-      </c>
-      <c r="F22" s="3">
-        <v>310396.5</v>
-      </c>
-      <c r="G22" s="3">
-        <v>266774.25</v>
-      </c>
-      <c r="H22" s="3">
-        <v>304310.08333333331</v>
-      </c>
-      <c r="I22" s="3">
-        <v>312073.91666666669</v>
-      </c>
-      <c r="J22" s="3">
-        <v>324577.58333333331</v>
-      </c>
-      <c r="K22" s="3">
-        <v>345739.08333333331</v>
-      </c>
-      <c r="L22" s="3">
-        <v>406106.5</v>
-      </c>
-      <c r="M22" s="3">
-        <v>438002.58333333331</v>
-      </c>
-      <c r="N22" s="3">
-        <v>483333.41666666669</v>
-      </c>
-      <c r="O22" s="3">
-        <v>492318.58333333331</v>
-      </c>
-      <c r="P22" s="3">
-        <v>497090.91666666669</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>487389.66666666669</v>
+      <c r="E22" s="4">
+        <v>306229</v>
+      </c>
+      <c r="F22" s="4">
+        <v>310397</v>
+      </c>
+      <c r="G22" s="4">
+        <v>266774</v>
+      </c>
+      <c r="H22" s="4">
+        <v>304310</v>
+      </c>
+      <c r="I22" s="4">
+        <v>312074</v>
+      </c>
+      <c r="J22" s="4">
+        <v>324578</v>
+      </c>
+      <c r="K22" s="4">
+        <v>345739</v>
+      </c>
+      <c r="L22" s="4">
+        <v>406107</v>
+      </c>
+      <c r="M22" s="4">
+        <v>438003</v>
+      </c>
+      <c r="N22" s="4">
+        <v>483333</v>
+      </c>
+      <c r="O22" s="4">
+        <v>492319</v>
+      </c>
+      <c r="P22" s="4">
+        <v>497091</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>487390</v>
       </c>
       <c r="GO22" s="1"/>
     </row>
@@ -1902,53 +1907,53 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>221888.91666666666</v>
-      </c>
-      <c r="C23" s="3">
-        <v>228852.91666666666</v>
-      </c>
-      <c r="D23" s="3">
-        <v>250142.5</v>
-      </c>
-      <c r="E23" s="3">
-        <v>298235.25</v>
-      </c>
-      <c r="F23" s="3">
-        <v>295475.83333333331</v>
-      </c>
-      <c r="G23" s="3">
-        <v>267337.16666666669</v>
-      </c>
-      <c r="H23" s="3">
-        <v>297167.83333333331</v>
-      </c>
-      <c r="I23" s="3">
-        <v>304029.91666666669</v>
-      </c>
-      <c r="J23" s="3">
-        <v>327465.83333333331</v>
-      </c>
-      <c r="K23" s="3">
-        <v>362965.66666666669</v>
-      </c>
-      <c r="L23" s="3">
-        <v>433624.83333333331</v>
-      </c>
-      <c r="M23" s="3">
+      <c r="B23" s="4">
+        <v>221889</v>
+      </c>
+      <c r="C23" s="4">
+        <v>228853</v>
+      </c>
+      <c r="D23" s="4">
+        <v>250143</v>
+      </c>
+      <c r="E23" s="4">
+        <v>298235</v>
+      </c>
+      <c r="F23" s="4">
+        <v>295476</v>
+      </c>
+      <c r="G23" s="4">
+        <v>267337</v>
+      </c>
+      <c r="H23" s="4">
+        <v>297168</v>
+      </c>
+      <c r="I23" s="4">
+        <v>304030</v>
+      </c>
+      <c r="J23" s="4">
+        <v>327466</v>
+      </c>
+      <c r="K23" s="4">
+        <v>362966</v>
+      </c>
+      <c r="L23" s="4">
+        <v>433625</v>
+      </c>
+      <c r="M23" s="4">
         <v>471614</v>
       </c>
-      <c r="N23" s="3">
-        <v>514562.33333333331</v>
-      </c>
-      <c r="O23" s="3">
-        <v>518503.58333333331</v>
-      </c>
-      <c r="P23" s="3">
-        <v>511536.41666666669</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>508148.91666666669</v>
+      <c r="N23" s="4">
+        <v>514562</v>
+      </c>
+      <c r="O23" s="4">
+        <v>518504</v>
+      </c>
+      <c r="P23" s="4">
+        <v>511536</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>508149</v>
       </c>
       <c r="GO23" s="1"/>
     </row>
@@ -1956,53 +1961,53 @@
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>184058.5</v>
-      </c>
-      <c r="C24" s="3">
-        <v>190867.83333333334</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="B24" s="4">
+        <v>184059</v>
+      </c>
+      <c r="C24" s="4">
+        <v>190868</v>
+      </c>
+      <c r="D24" s="4">
         <v>202362</v>
       </c>
-      <c r="E24" s="3">
-        <v>229655.41666666666</v>
-      </c>
-      <c r="F24" s="3">
-        <v>231283.58333333334</v>
-      </c>
-      <c r="G24" s="3">
-        <v>211307.5</v>
-      </c>
-      <c r="H24" s="3">
-        <v>225582.16666666666</v>
-      </c>
-      <c r="I24" s="3">
-        <v>228017.5</v>
-      </c>
-      <c r="J24" s="3">
+      <c r="E24" s="4">
+        <v>229655</v>
+      </c>
+      <c r="F24" s="4">
+        <v>231284</v>
+      </c>
+      <c r="G24" s="4">
+        <v>211308</v>
+      </c>
+      <c r="H24" s="4">
+        <v>225582</v>
+      </c>
+      <c r="I24" s="4">
+        <v>228018</v>
+      </c>
+      <c r="J24" s="4">
         <v>240572</v>
       </c>
-      <c r="K24" s="3">
-        <v>260815.08333333334</v>
-      </c>
-      <c r="L24" s="3">
-        <v>315812.58333333331</v>
-      </c>
-      <c r="M24" s="3">
-        <v>355049.91666666669</v>
-      </c>
-      <c r="N24" s="3">
-        <v>402648.66666666669</v>
-      </c>
-      <c r="O24" s="3">
-        <v>411048.91666666669</v>
-      </c>
-      <c r="P24" s="3">
-        <v>411628.83333333331</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>409791.16666666669</v>
+      <c r="K24" s="4">
+        <v>260815</v>
+      </c>
+      <c r="L24" s="4">
+        <v>315813</v>
+      </c>
+      <c r="M24" s="4">
+        <v>355050</v>
+      </c>
+      <c r="N24" s="4">
+        <v>402649</v>
+      </c>
+      <c r="O24" s="4">
+        <v>411049</v>
+      </c>
+      <c r="P24" s="4">
+        <v>411629</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>409791</v>
       </c>
       <c r="GO24" s="1"/>
     </row>
@@ -2010,53 +2015,53 @@
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
-        <v>238098.75</v>
-      </c>
-      <c r="C25" s="3">
-        <v>246252.91666666666</v>
-      </c>
-      <c r="D25" s="3">
-        <v>257060.66666666666</v>
-      </c>
-      <c r="E25" s="3">
-        <v>297858.5</v>
-      </c>
-      <c r="F25" s="3">
-        <v>300674.5</v>
-      </c>
-      <c r="G25" s="3">
-        <v>271598.16666666669</v>
-      </c>
-      <c r="H25" s="3">
-        <v>299999.33333333331</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="B25" s="4">
+        <v>238099</v>
+      </c>
+      <c r="C25" s="4">
+        <v>246253</v>
+      </c>
+      <c r="D25" s="4">
+        <v>257061</v>
+      </c>
+      <c r="E25" s="4">
+        <v>297859</v>
+      </c>
+      <c r="F25" s="4">
+        <v>300675</v>
+      </c>
+      <c r="G25" s="4">
+        <v>271598</v>
+      </c>
+      <c r="H25" s="4">
+        <v>299999</v>
+      </c>
+      <c r="I25" s="4">
         <v>306063</v>
       </c>
-      <c r="J25" s="3">
-        <v>316742.83333333331</v>
-      </c>
-      <c r="K25" s="3">
-        <v>344544.33333333331</v>
-      </c>
-      <c r="L25" s="3">
-        <v>419976.83333333331</v>
-      </c>
-      <c r="M25" s="3">
-        <v>457702.25</v>
-      </c>
-      <c r="N25" s="3">
-        <v>500267.41666666669</v>
-      </c>
-      <c r="O25" s="3">
-        <v>512185.83333333331</v>
-      </c>
-      <c r="P25" s="3">
-        <v>512293.91666666669</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>507355.83333333331</v>
+      <c r="J25" s="4">
+        <v>316743</v>
+      </c>
+      <c r="K25" s="4">
+        <v>344544</v>
+      </c>
+      <c r="L25" s="4">
+        <v>419977</v>
+      </c>
+      <c r="M25" s="4">
+        <v>457702</v>
+      </c>
+      <c r="N25" s="4">
+        <v>500267</v>
+      </c>
+      <c r="O25" s="4">
+        <v>512186</v>
+      </c>
+      <c r="P25" s="4">
+        <v>512294</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>507356</v>
       </c>
       <c r="GO25" s="1"/>
     </row>
@@ -2064,53 +2069,53 @@
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
-        <v>185680.33333333334</v>
-      </c>
-      <c r="C26" s="3">
-        <v>193555.33333333334</v>
-      </c>
-      <c r="D26" s="3">
-        <v>203284.75</v>
-      </c>
-      <c r="E26" s="3">
-        <v>226388.58333333334</v>
-      </c>
-      <c r="F26" s="3">
-        <v>221768.41666666666</v>
-      </c>
-      <c r="G26" s="3">
-        <v>188217.33333333334</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="B26" s="4">
+        <v>185680</v>
+      </c>
+      <c r="C26" s="4">
+        <v>193555</v>
+      </c>
+      <c r="D26" s="4">
+        <v>203285</v>
+      </c>
+      <c r="E26" s="4">
+        <v>226389</v>
+      </c>
+      <c r="F26" s="4">
+        <v>221768</v>
+      </c>
+      <c r="G26" s="4">
+        <v>188217</v>
+      </c>
+      <c r="H26" s="4">
         <v>204467</v>
       </c>
-      <c r="I26" s="3">
-        <v>207663.5</v>
-      </c>
-      <c r="J26" s="3">
-        <v>212824.75</v>
-      </c>
-      <c r="K26" s="3">
-        <v>222784.16666666666</v>
-      </c>
-      <c r="L26" s="3">
-        <v>258312.25</v>
-      </c>
-      <c r="M26" s="3">
-        <v>297558.08333333331</v>
-      </c>
-      <c r="N26" s="3">
-        <v>347956.91666666669</v>
-      </c>
-      <c r="O26" s="3">
-        <v>362131.5</v>
-      </c>
-      <c r="P26" s="3">
-        <v>359022.5</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>364072.25</v>
+      <c r="I26" s="4">
+        <v>207664</v>
+      </c>
+      <c r="J26" s="4">
+        <v>212825</v>
+      </c>
+      <c r="K26" s="4">
+        <v>222784</v>
+      </c>
+      <c r="L26" s="4">
+        <v>258312</v>
+      </c>
+      <c r="M26" s="4">
+        <v>297558</v>
+      </c>
+      <c r="N26" s="4">
+        <v>347957</v>
+      </c>
+      <c r="O26" s="4">
+        <v>362132</v>
+      </c>
+      <c r="P26" s="4">
+        <v>359023</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>364072</v>
       </c>
       <c r="GO26" s="1"/>
     </row>
@@ -2118,53 +2123,53 @@
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
-        <v>222917.66666666666</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="B27" s="4">
+        <v>222918</v>
+      </c>
+      <c r="C27" s="4">
         <v>226469</v>
       </c>
-      <c r="D27" s="3">
-        <v>239729.66666666666</v>
-      </c>
-      <c r="E27" s="3">
-        <v>266937.75</v>
-      </c>
-      <c r="F27" s="3">
-        <v>264429.41666666669</v>
-      </c>
-      <c r="G27" s="3">
-        <v>232764.08333333334</v>
-      </c>
-      <c r="H27" s="3">
-        <v>252334.41666666666</v>
-      </c>
-      <c r="I27" s="3">
-        <v>261965.5</v>
-      </c>
-      <c r="J27" s="3">
+      <c r="D27" s="4">
+        <v>239730</v>
+      </c>
+      <c r="E27" s="4">
+        <v>266938</v>
+      </c>
+      <c r="F27" s="4">
+        <v>264429</v>
+      </c>
+      <c r="G27" s="4">
+        <v>232764</v>
+      </c>
+      <c r="H27" s="4">
+        <v>252334</v>
+      </c>
+      <c r="I27" s="4">
+        <v>261966</v>
+      </c>
+      <c r="J27" s="4">
         <v>265912</v>
       </c>
-      <c r="K27" s="3">
-        <v>274824.91666666669</v>
-      </c>
-      <c r="L27" s="3">
-        <v>304162.41666666669</v>
-      </c>
-      <c r="M27" s="3">
-        <v>343795.33333333331</v>
-      </c>
-      <c r="N27" s="3">
-        <v>391837.25</v>
-      </c>
-      <c r="O27" s="3">
-        <v>410300.16666666669</v>
-      </c>
-      <c r="P27" s="3">
-        <v>422591.25</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>413412.16666666669</v>
+      <c r="K27" s="4">
+        <v>274825</v>
+      </c>
+      <c r="L27" s="4">
+        <v>304162</v>
+      </c>
+      <c r="M27" s="4">
+        <v>343795</v>
+      </c>
+      <c r="N27" s="4">
+        <v>391837</v>
+      </c>
+      <c r="O27" s="4">
+        <v>410300</v>
+      </c>
+      <c r="P27" s="4">
+        <v>422591</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>413412</v>
       </c>
       <c r="GO27" s="1"/>
     </row>
@@ -2172,53 +2177,53 @@
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>316541</v>
       </c>
-      <c r="C28" s="3">
-        <v>323618.91666666669</v>
-      </c>
-      <c r="D28" s="3">
-        <v>348496.75</v>
-      </c>
-      <c r="E28" s="3">
-        <v>410382.75</v>
-      </c>
-      <c r="F28" s="3">
-        <v>409389.08333333331</v>
-      </c>
-      <c r="G28" s="3">
-        <v>369390.25</v>
-      </c>
-      <c r="H28" s="3">
-        <v>420083.58333333331</v>
-      </c>
-      <c r="I28" s="3">
-        <v>434537.08333333331</v>
-      </c>
-      <c r="J28" s="3">
-        <v>454941.83333333331</v>
-      </c>
-      <c r="K28" s="3">
-        <v>492115.66666666669</v>
-      </c>
-      <c r="L28" s="3">
-        <v>577055.33333333337</v>
-      </c>
-      <c r="M28" s="3">
+      <c r="C28" s="4">
+        <v>323619</v>
+      </c>
+      <c r="D28" s="4">
+        <v>348497</v>
+      </c>
+      <c r="E28" s="4">
+        <v>410383</v>
+      </c>
+      <c r="F28" s="4">
+        <v>409389</v>
+      </c>
+      <c r="G28" s="4">
+        <v>369390</v>
+      </c>
+      <c r="H28" s="4">
+        <v>420084</v>
+      </c>
+      <c r="I28" s="4">
+        <v>434537</v>
+      </c>
+      <c r="J28" s="4">
+        <v>454942</v>
+      </c>
+      <c r="K28" s="4">
+        <v>492116</v>
+      </c>
+      <c r="L28" s="4">
+        <v>577055</v>
+      </c>
+      <c r="M28" s="4">
         <v>618778</v>
       </c>
-      <c r="N28" s="3">
-        <v>653760.75</v>
-      </c>
-      <c r="O28" s="3">
-        <v>665284.66666666663</v>
-      </c>
-      <c r="P28" s="3">
-        <v>652665.5</v>
-      </c>
-      <c r="Q28" s="3">
-        <v>650341.5</v>
+      <c r="N28" s="4">
+        <v>653761</v>
+      </c>
+      <c r="O28" s="4">
+        <v>665285</v>
+      </c>
+      <c r="P28" s="4">
+        <v>652666</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>650342</v>
       </c>
       <c r="GO28" s="1"/>
     </row>
@@ -2226,53 +2231,53 @@
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>216903.91666666666</v>
-      </c>
-      <c r="C29" s="3">
-        <v>224050.25</v>
-      </c>
-      <c r="D29" s="3">
-        <v>242759.66666666666</v>
-      </c>
-      <c r="E29" s="3">
-        <v>289668.16666666669</v>
-      </c>
-      <c r="F29" s="3">
-        <v>291213.25</v>
-      </c>
-      <c r="G29" s="3">
-        <v>261151.08333333334</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="B29" s="4">
+        <v>216904</v>
+      </c>
+      <c r="C29" s="4">
+        <v>224050</v>
+      </c>
+      <c r="D29" s="4">
+        <v>242760</v>
+      </c>
+      <c r="E29" s="4">
+        <v>289668</v>
+      </c>
+      <c r="F29" s="4">
+        <v>291213</v>
+      </c>
+      <c r="G29" s="4">
+        <v>261151</v>
+      </c>
+      <c r="H29" s="4">
         <v>293913</v>
       </c>
-      <c r="I29" s="3">
-        <v>312539.58333333331</v>
-      </c>
-      <c r="J29" s="3">
-        <v>331124.16666666669</v>
-      </c>
-      <c r="K29" s="3">
-        <v>360749.83333333331</v>
-      </c>
-      <c r="L29" s="3">
-        <v>427767.5</v>
-      </c>
-      <c r="M29" s="3">
-        <v>467867.58333333331</v>
-      </c>
-      <c r="N29" s="3">
-        <v>510331.33333333331</v>
-      </c>
-      <c r="O29" s="3">
-        <v>515883.33333333331</v>
-      </c>
-      <c r="P29" s="3">
-        <v>504235.25</v>
-      </c>
-      <c r="Q29" s="3">
-        <v>499192.41666666669</v>
+      <c r="I29" s="4">
+        <v>312540</v>
+      </c>
+      <c r="J29" s="4">
+        <v>331124</v>
+      </c>
+      <c r="K29" s="4">
+        <v>360750</v>
+      </c>
+      <c r="L29" s="4">
+        <v>427768</v>
+      </c>
+      <c r="M29" s="4">
+        <v>467868</v>
+      </c>
+      <c r="N29" s="4">
+        <v>510331</v>
+      </c>
+      <c r="O29" s="4">
+        <v>515883</v>
+      </c>
+      <c r="P29" s="4">
+        <v>504235</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>499192</v>
       </c>
       <c r="GO29" s="1"/>
     </row>
@@ -2280,53 +2285,53 @@
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>201829.25</v>
-      </c>
-      <c r="C30" s="3">
-        <v>209547.25</v>
-      </c>
-      <c r="D30" s="3">
-        <v>215723.83333333334</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="B30" s="4">
+        <v>201829</v>
+      </c>
+      <c r="C30" s="4">
+        <v>209547</v>
+      </c>
+      <c r="D30" s="4">
+        <v>215724</v>
+      </c>
+      <c r="E30" s="4">
         <v>241438</v>
       </c>
-      <c r="F30" s="3">
-        <v>242701.91666666666</v>
-      </c>
-      <c r="G30" s="3">
-        <v>212117.75</v>
-      </c>
-      <c r="H30" s="3">
-        <v>233489.41666666666</v>
-      </c>
-      <c r="I30" s="3">
-        <v>233026.75</v>
-      </c>
-      <c r="J30" s="3">
-        <v>238842.16666666666</v>
-      </c>
-      <c r="K30" s="3">
-        <v>252002.75</v>
-      </c>
-      <c r="L30" s="3">
-        <v>291132.16666666669</v>
-      </c>
-      <c r="M30" s="3">
-        <v>322932.25</v>
-      </c>
-      <c r="N30" s="3">
-        <v>365303.08333333331</v>
-      </c>
-      <c r="O30" s="3">
-        <v>376924.5</v>
-      </c>
-      <c r="P30" s="3">
-        <v>379262.58333333331</v>
-      </c>
-      <c r="Q30" s="3">
-        <v>372501.08333333331</v>
+      <c r="F30" s="4">
+        <v>242702</v>
+      </c>
+      <c r="G30" s="4">
+        <v>212118</v>
+      </c>
+      <c r="H30" s="4">
+        <v>233489</v>
+      </c>
+      <c r="I30" s="4">
+        <v>233027</v>
+      </c>
+      <c r="J30" s="4">
+        <v>238842</v>
+      </c>
+      <c r="K30" s="4">
+        <v>252003</v>
+      </c>
+      <c r="L30" s="4">
+        <v>291132</v>
+      </c>
+      <c r="M30" s="4">
+        <v>322932</v>
+      </c>
+      <c r="N30" s="4">
+        <v>365303</v>
+      </c>
+      <c r="O30" s="4">
+        <v>376925</v>
+      </c>
+      <c r="P30" s="4">
+        <v>379263</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>372501</v>
       </c>
       <c r="GO30" s="1"/>
     </row>
@@ -2334,53 +2339,53 @@
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>219986.91666666666</v>
-      </c>
-      <c r="C31" s="3">
-        <v>225628.91666666666</v>
-      </c>
-      <c r="D31" s="3">
-        <v>243033.08333333334</v>
-      </c>
-      <c r="E31" s="3">
-        <v>287172.83333333331</v>
-      </c>
-      <c r="F31" s="3">
-        <v>298002.16666666669</v>
-      </c>
-      <c r="G31" s="3">
-        <v>258248.41666666666</v>
-      </c>
-      <c r="H31" s="3">
-        <v>282748.75</v>
-      </c>
-      <c r="I31" s="3">
-        <v>287262.41666666669</v>
-      </c>
-      <c r="J31" s="3">
+      <c r="B31" s="4">
+        <v>219987</v>
+      </c>
+      <c r="C31" s="4">
+        <v>225629</v>
+      </c>
+      <c r="D31" s="4">
+        <v>243033</v>
+      </c>
+      <c r="E31" s="4">
+        <v>287173</v>
+      </c>
+      <c r="F31" s="4">
+        <v>298002</v>
+      </c>
+      <c r="G31" s="4">
+        <v>258248</v>
+      </c>
+      <c r="H31" s="4">
+        <v>282749</v>
+      </c>
+      <c r="I31" s="4">
+        <v>287262</v>
+      </c>
+      <c r="J31" s="4">
         <v>285453</v>
       </c>
-      <c r="K31" s="3">
-        <v>309051.08333333331</v>
-      </c>
-      <c r="L31" s="3">
-        <v>382241.66666666669</v>
-      </c>
-      <c r="M31" s="3">
+      <c r="K31" s="4">
+        <v>309051</v>
+      </c>
+      <c r="L31" s="4">
+        <v>382242</v>
+      </c>
+      <c r="M31" s="4">
         <v>421944</v>
       </c>
-      <c r="N31" s="3">
-        <v>457129.58333333331</v>
-      </c>
-      <c r="O31" s="3">
+      <c r="N31" s="4">
+        <v>457130</v>
+      </c>
+      <c r="O31" s="4">
         <v>459279</v>
       </c>
-      <c r="P31" s="3">
-        <v>446500.41666666669</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>439009.58333333331</v>
+      <c r="P31" s="4">
+        <v>446500</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>439010</v>
       </c>
       <c r="GO31" s="1"/>
     </row>
@@ -2388,53 +2393,53 @@
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>191377.75</v>
-      </c>
-      <c r="C32" s="3">
-        <v>197240.5</v>
-      </c>
-      <c r="D32" s="3">
-        <v>209707.75</v>
-      </c>
-      <c r="E32" s="3">
-        <v>237017.33333333334</v>
-      </c>
-      <c r="F32" s="3">
-        <v>232886.5</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="B32" s="4">
+        <v>191378</v>
+      </c>
+      <c r="C32" s="4">
+        <v>197241</v>
+      </c>
+      <c r="D32" s="4">
+        <v>209708</v>
+      </c>
+      <c r="E32" s="4">
+        <v>237017</v>
+      </c>
+      <c r="F32" s="4">
+        <v>232887</v>
+      </c>
+      <c r="G32" s="4">
         <v>204935</v>
       </c>
-      <c r="H32" s="3">
-        <v>222102.25</v>
-      </c>
-      <c r="I32" s="3">
-        <v>220905.41666666666</v>
-      </c>
-      <c r="J32" s="3">
-        <v>230726.66666666666</v>
-      </c>
-      <c r="K32" s="3">
-        <v>254265.25</v>
-      </c>
-      <c r="L32" s="3">
-        <v>314934.25</v>
-      </c>
-      <c r="M32" s="3">
-        <v>357513.33333333331</v>
-      </c>
-      <c r="N32" s="3">
-        <v>413149.41666666669</v>
-      </c>
-      <c r="O32" s="3">
-        <v>436116.58333333331</v>
-      </c>
-      <c r="P32" s="3">
-        <v>440859.41666666669</v>
-      </c>
-      <c r="Q32" s="3">
-        <v>430663.58333333331</v>
+      <c r="H32" s="4">
+        <v>222102</v>
+      </c>
+      <c r="I32" s="4">
+        <v>220905</v>
+      </c>
+      <c r="J32" s="4">
+        <v>230727</v>
+      </c>
+      <c r="K32" s="4">
+        <v>254265</v>
+      </c>
+      <c r="L32" s="4">
+        <v>314934</v>
+      </c>
+      <c r="M32" s="4">
+        <v>357513</v>
+      </c>
+      <c r="N32" s="4">
+        <v>413149</v>
+      </c>
+      <c r="O32" s="4">
+        <v>436117</v>
+      </c>
+      <c r="P32" s="4">
+        <v>440859</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>430664</v>
       </c>
       <c r="GO32" s="1"/>
     </row>
@@ -2442,53 +2447,53 @@
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>271649.66666666669</v>
-      </c>
-      <c r="C33" s="3">
+      <c r="B33" s="4">
+        <v>271650</v>
+      </c>
+      <c r="C33" s="4">
         <v>284182</v>
       </c>
-      <c r="D33" s="3">
-        <v>310943.91666666669</v>
-      </c>
-      <c r="E33" s="3">
-        <v>372077.41666666669</v>
-      </c>
-      <c r="F33" s="3">
-        <v>363817.5</v>
-      </c>
-      <c r="G33" s="3">
-        <v>340373.16666666669</v>
-      </c>
-      <c r="H33" s="3">
-        <v>374487.91666666669</v>
-      </c>
-      <c r="I33" s="3">
-        <v>386200.08333333331</v>
-      </c>
-      <c r="J33" s="3">
-        <v>409392.08333333331</v>
-      </c>
-      <c r="K33" s="3">
+      <c r="D33" s="4">
+        <v>310944</v>
+      </c>
+      <c r="E33" s="4">
+        <v>372077</v>
+      </c>
+      <c r="F33" s="4">
+        <v>363818</v>
+      </c>
+      <c r="G33" s="4">
+        <v>340373</v>
+      </c>
+      <c r="H33" s="4">
+        <v>374488</v>
+      </c>
+      <c r="I33" s="4">
+        <v>386200</v>
+      </c>
+      <c r="J33" s="4">
+        <v>409392</v>
+      </c>
+      <c r="K33" s="4">
         <v>457404</v>
       </c>
-      <c r="L33" s="3">
-        <v>544515.08333333337</v>
-      </c>
-      <c r="M33" s="3">
-        <v>572691.25</v>
-      </c>
-      <c r="N33" s="3">
-        <v>608740.83333333337</v>
-      </c>
-      <c r="O33" s="3">
-        <v>617921.41666666663</v>
-      </c>
-      <c r="P33" s="3">
-        <v>596649.16666666663</v>
-      </c>
-      <c r="Q33" s="3">
-        <v>588672.41666666663</v>
+      <c r="L33" s="4">
+        <v>544515</v>
+      </c>
+      <c r="M33" s="4">
+        <v>572691</v>
+      </c>
+      <c r="N33" s="4">
+        <v>608741</v>
+      </c>
+      <c r="O33" s="4">
+        <v>617921</v>
+      </c>
+      <c r="P33" s="4">
+        <v>596649</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>588672</v>
       </c>
       <c r="GO33" s="1"/>
     </row>
@@ -2496,52 +2501,52 @@
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
-        <v>379395.33333333331</v>
-      </c>
-      <c r="C34" s="3">
+      <c r="B34" s="4">
+        <v>379395</v>
+      </c>
+      <c r="C34" s="4">
         <v>399385</v>
       </c>
-      <c r="D34" s="3">
-        <v>436864.75</v>
-      </c>
-      <c r="E34" s="3">
-        <v>514426.58333333331</v>
-      </c>
-      <c r="F34" s="3">
-        <v>540196.75</v>
-      </c>
-      <c r="G34" s="3">
-        <v>532096.83333333337</v>
-      </c>
-      <c r="H34" s="3">
-        <v>606698.33333333337</v>
-      </c>
-      <c r="I34" s="3">
-        <v>632513.58333333337</v>
-      </c>
-      <c r="J34" s="3">
-        <v>696926.08333333337</v>
-      </c>
-      <c r="K34" s="3">
-        <v>789972.5</v>
-      </c>
-      <c r="L34" s="3">
-        <v>922702.16666666663</v>
-      </c>
-      <c r="M34" s="3">
+      <c r="D34" s="4">
+        <v>436865</v>
+      </c>
+      <c r="E34" s="4">
+        <v>514427</v>
+      </c>
+      <c r="F34" s="4">
+        <v>540197</v>
+      </c>
+      <c r="G34" s="4">
+        <v>532097</v>
+      </c>
+      <c r="H34" s="4">
+        <v>606698</v>
+      </c>
+      <c r="I34" s="4">
+        <v>632514</v>
+      </c>
+      <c r="J34" s="4">
+        <v>696926</v>
+      </c>
+      <c r="K34" s="4">
+        <v>789973</v>
+      </c>
+      <c r="L34" s="4">
+        <v>922702</v>
+      </c>
+      <c r="M34" s="4">
         <v>964643</v>
       </c>
-      <c r="N34" s="3">
-        <v>995543.33333333337</v>
-      </c>
-      <c r="O34" s="3">
-        <v>1064771.5</v>
-      </c>
-      <c r="P34" s="3">
-        <v>1020025.5</v>
-      </c>
-      <c r="Q34" s="3">
+      <c r="N34" s="4">
+        <v>995543</v>
+      </c>
+      <c r="O34" s="4">
+        <v>1064772</v>
+      </c>
+      <c r="P34" s="4">
+        <v>1020026</v>
+      </c>
+      <c r="Q34" s="4">
         <v>958304</v>
       </c>
       <c r="GO34" s="1"/>
@@ -2550,53 +2555,53 @@
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
-        <v>228614.08333333334</v>
-      </c>
-      <c r="C35" s="3">
-        <v>235329.33333333334</v>
-      </c>
-      <c r="D35" s="3">
-        <v>251281.16666666666</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="B35" s="4">
+        <v>228614</v>
+      </c>
+      <c r="C35" s="4">
+        <v>235329</v>
+      </c>
+      <c r="D35" s="4">
+        <v>251281</v>
+      </c>
+      <c r="E35" s="4">
         <v>287114</v>
       </c>
-      <c r="F35" s="3">
-        <v>282958.83333333331</v>
-      </c>
-      <c r="G35" s="3">
-        <v>257853.91666666666</v>
-      </c>
-      <c r="H35" s="3">
-        <v>284543.16666666669</v>
-      </c>
-      <c r="I35" s="3">
-        <v>290551.16666666669</v>
-      </c>
-      <c r="J35" s="3">
-        <v>303927.33333333331</v>
-      </c>
-      <c r="K35" s="3">
-        <v>329167.75</v>
-      </c>
-      <c r="L35" s="3">
-        <v>386124.33333333331</v>
-      </c>
-      <c r="M35" s="3">
-        <v>425134.08333333331</v>
-      </c>
-      <c r="N35" s="3">
-        <v>467502.91666666669</v>
-      </c>
-      <c r="O35" s="3">
-        <v>480247.25</v>
-      </c>
-      <c r="P35" s="3">
-        <v>477854.75</v>
-      </c>
-      <c r="Q35" s="3">
-        <v>471785.08333333331</v>
+      <c r="F35" s="4">
+        <v>282959</v>
+      </c>
+      <c r="G35" s="4">
+        <v>257854</v>
+      </c>
+      <c r="H35" s="4">
+        <v>284543</v>
+      </c>
+      <c r="I35" s="4">
+        <v>290551</v>
+      </c>
+      <c r="J35" s="4">
+        <v>303927</v>
+      </c>
+      <c r="K35" s="4">
+        <v>329168</v>
+      </c>
+      <c r="L35" s="4">
+        <v>386124</v>
+      </c>
+      <c r="M35" s="4">
+        <v>425134</v>
+      </c>
+      <c r="N35" s="4">
+        <v>467503</v>
+      </c>
+      <c r="O35" s="4">
+        <v>480247</v>
+      </c>
+      <c r="P35" s="4">
+        <v>477855</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>471785</v>
       </c>
       <c r="GO35" s="1"/>
     </row>
@@ -3993,5 +3998,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>